<commit_message>
change architecture  ( in progress )
</commit_message>
<xml_diff>
--- a/test/Fixture/DataAccessor/Sample.xlsx
+++ b/test/Fixture/DataAccessor/Sample.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="24990" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="24990"/>
   </bookViews>
   <sheets>
     <sheet name="Quest" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,39 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+  <si>
+    <t>id1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>attr1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>attr2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>attr3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -349,14 +382,215 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+      <c r="F7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>3</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+      <c r="F9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="D10">
+        <v>3</v>
+      </c>
+      <c r="E10">
+        <v>3</v>
+      </c>
+      <c r="F10">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -366,12 +600,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>